<commit_message>
Added 5.3.3.1 data (screen shots)
</commit_message>
<xml_diff>
--- a/Wire-chenber/Ex.1/5.9keV-calc.xlsx
+++ b/Wire-chenber/Ex.1/5.9keV-calc.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuichimori/Experiment_III/Wire-chenber/Ex.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A693D5BC-5081-1142-BD7F-240F23C92F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC1A4BB-0492-3F45-B229-FD6F568CBE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DF0F2A2E-BA8D-A249-AB36-14773BE9531C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{DF0F2A2E-BA8D-A249-AB36-14773BE9531C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>5.9keV</t>
     <phoneticPr fontId="1"/>
@@ -129,6 +129,46 @@
   </si>
   <si>
     <t>C.(2)*</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C.(5)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3keV</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>吸収係数/cm</t>
+    <rPh sb="0" eb="4">
+      <t>キュウシュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>電子質量(MeV)</t>
+    <rPh sb="0" eb="4">
+      <t>デンセィ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">D(1) </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">運動エネルギーT (MeV) </t>
+    <rPh sb="0" eb="2">
+      <t>ウンドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>速度</t>
+    <rPh sb="0" eb="2">
+      <t>ソクド</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3308,21 +3348,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A51087-2FFC-5040-B149-EFF974C73FD6}">
-  <dimension ref="B2:O32"/>
+  <dimension ref="A2:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="93" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14">
+    <row r="2" spans="1:14">
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3342,7 +3383,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="3:14">
+    <row r="3" spans="1:14">
       <c r="C3">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3362,7 +3403,7 @@
         <v>757.1</v>
       </c>
     </row>
-    <row r="4" spans="3:14">
+    <row r="4" spans="1:14">
       <c r="C4">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3382,7 +3423,7 @@
         <v>422.5</v>
       </c>
     </row>
-    <row r="5" spans="3:14">
+    <row r="5" spans="1:14">
       <c r="C5">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -3402,7 +3443,7 @@
         <v>259.39999999999998</v>
       </c>
     </row>
-    <row r="6" spans="3:14">
+    <row r="6" spans="1:14">
       <c r="C6">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -3420,6 +3461,16 @@
       </c>
       <c r="M6">
         <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>0.51</v>
       </c>
     </row>
     <row r="25" spans="2:15">
@@ -3558,6 +3609,19 @@
       <c r="H31" t="s">
         <v>18</v>
       </c>
+      <c r="K31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31">
+        <f>4394.3*EXP(-458.6*0.003)</f>
+        <v>1110.1645488583022</v>
+      </c>
+      <c r="N31" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="2:15">
       <c r="F32" t="s">
@@ -3569,6 +3633,74 @@
       <c r="H32">
         <f>EXP(-H28*G31/10000)</f>
         <v>0.67591754954087691</v>
+      </c>
+      <c r="L32" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32">
+        <f>M31*M27</f>
+        <v>1.976092896967778</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="L33" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33">
+        <f>1/M32</f>
+        <v>0.506049083792798</v>
+      </c>
+      <c r="N33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37">
+        <v>0.5</v>
+      </c>
+      <c r="C37">
+        <f>SQRT(1-($A$14/(B37+$A$14))^2)</f>
+        <v>0.86314830565161849</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ref="C38:C40" si="0">SQRT(1-($A$14/(B38+$A$14))^2)</f>
+        <v>0.94123645056635075</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39">
+        <v>1.5</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>0.96727473110565076</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>0.97913989860115602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started preparing for the report
</commit_message>
<xml_diff>
--- a/Wire-chenber/Ex.1/5.9keV-calc.xlsx
+++ b/Wire-chenber/Ex.1/5.9keV-calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuichimori/Experiment_III/Wire-chenber/Ex.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC1A4BB-0492-3F45-B229-FD6F568CBE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55F6ED1-E96C-7648-8904-4C2822CD15F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{DF0F2A2E-BA8D-A249-AB36-14773BE9531C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DF0F2A2E-BA8D-A249-AB36-14773BE9531C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>5.9keV</t>
     <phoneticPr fontId="1"/>
@@ -169,6 +169,33 @@
     <rPh sb="0" eb="2">
       <t>ソクド</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>βγ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D(2)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dE/dx|min (MeVg^{-1}cm^2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">density (gcm^{-3}) </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">距離 (cm) </t>
+    <rPh sb="0" eb="2">
+      <t>キョリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(MeV)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3348,16 +3375,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A51087-2FFC-5040-B149-EFF974C73FD6}">
-  <dimension ref="A2:O40"/>
+  <dimension ref="A2:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="93" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
@@ -3666,6 +3693,9 @@
       <c r="C36" t="s">
         <v>26</v>
       </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="37" spans="2:14">
       <c r="B37">
@@ -3675,6 +3705,10 @@
         <f>SQRT(1-($A$14/(B37+$A$14))^2)</f>
         <v>0.86314830565161849</v>
       </c>
+      <c r="D37">
+        <f>C37*B37/$A$14</f>
+        <v>0.84622382907021421</v>
+      </c>
     </row>
     <row r="38" spans="2:14">
       <c r="B38">
@@ -3684,6 +3718,10 @@
         <f t="shared" ref="C38:C40" si="0">SQRT(1-($A$14/(B38+$A$14))^2)</f>
         <v>0.94123645056635075</v>
       </c>
+      <c r="D38">
+        <f t="shared" ref="D38:D40" si="1">C38*B38/$A$14</f>
+        <v>1.8455616677771582</v>
+      </c>
     </row>
     <row r="39" spans="2:14">
       <c r="B39">
@@ -3693,6 +3731,10 @@
         <f t="shared" si="0"/>
         <v>0.96727473110565076</v>
       </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>2.8449256797225022</v>
+      </c>
     </row>
     <row r="40" spans="2:14">
       <c r="B40">
@@ -3701,6 +3743,52 @@
       <c r="C40">
         <f t="shared" si="0"/>
         <v>0.97913989860115602</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>3.8397643082398276</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14">
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43">
+        <f>B44*B48*B46</f>
+        <v>4.8772051999999988</v>
+      </c>
+      <c r="D43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="B44">
+        <v>1.5189999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14">
+      <c r="B46">
+        <v>1.3959999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14">
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14">
+      <c r="B48">
+        <v>2.2999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>